<commit_message>
Updated OpenSRA.py to run anaylsis + above_ground example
</commit_message>
<xml_diff>
--- a/param_dist/above_ground.xlsx
+++ b/param_dist/above_ground.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://slategeotech-my.sharepoint.com/personal/bzheng_slategeotech_com/Documents/CEC/OpenSRA/param_dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="381" documentId="8_{2987D35D-B7D5-480E-B7BB-5CC225CF1AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B0B6077-EAC6-4A2C-BBA1-1B735564D412}"/>
+  <xr:revisionPtr revIDLastSave="384" documentId="8_{2987D35D-B7D5-480E-B7BB-5CC225CF1AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9DE7593-DF76-4FDB-B831-D9B35CBC8624}"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="9000" windowWidth="23640" windowHeight="10395" activeTab="3" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="level1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="level3" sheetId="3" r:id="rId3"/>
     <sheet name="fixed" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="1000" iterateDelta="9.9999999999999995E-7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -136,9 +136,6 @@
     <t>subsystems: 2 for p2, 3 for p3, 4 for p4</t>
   </si>
   <si>
-    <t>unitness</t>
-  </si>
-  <si>
     <t>l_p6_sys23</t>
   </si>
   <si>
@@ -209,6 +206,9 @@
   </si>
   <si>
     <t>presence of stretch length for anchors: True/False</t>
+  </si>
+  <si>
+    <t>unitless</t>
   </si>
 </sst>
 </file>
@@ -669,7 +669,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -698,7 +698,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -785,7 +785,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -823,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
@@ -841,21 +841,21 @@
         <v>13800</v>
       </c>
       <c r="K9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
         <v>44</v>
-      </c>
-      <c r="B10" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -887,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12">
         <v>5.5</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -942,10 +942,10 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
         <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>53</v>
       </c>
       <c r="F13">
         <v>6.89</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -971,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1113,7 +1113,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1220,7 +1220,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -1258,7 +1258,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
@@ -1276,21 +1276,21 @@
         <v>13800</v>
       </c>
       <c r="K9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
         <v>44</v>
-      </c>
-      <c r="B10" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
@@ -1342,7 +1342,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -1351,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12">
         <v>5.5</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -1377,10 +1377,10 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
         <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>53</v>
       </c>
       <c r="F13">
         <v>6.89</v>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -1406,7 +1406,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1548,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -1693,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
@@ -1711,21 +1711,21 @@
         <v>13800</v>
       </c>
       <c r="K9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
         <v>44</v>
-      </c>
-      <c r="B10" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
@@ -1748,7 +1748,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -1757,7 +1757,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -1786,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12">
         <v>5.5</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -1812,10 +1812,10 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
         <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>53</v>
       </c>
       <c r="F13">
         <v>6.89</v>
@@ -1832,7 +1832,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -1841,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -1869,16 +1869,16 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1916,7 +1916,7 @@
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
         <v>29</v>
@@ -1936,12 +1936,12 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1950,10 +1950,10 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -1961,19 +1961,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -1981,19 +1981,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
         <v>55</v>
       </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>56</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>

</xml_diff>